<commit_message>
updated test code and predictions
</commit_message>
<xml_diff>
--- a/Lifetime Predictions.xlsx
+++ b/Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77730681-2A05-4F1E-9C4D-91016FB22712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58017E40-D2C4-45A2-A803-BC04076FA5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Playing At:  Los Angeles Kings   Home</t>
+  </si>
+  <si>
+    <t>70% or greater</t>
+  </si>
+  <si>
+    <t>less than 70%</t>
   </si>
 </sst>
 </file>
@@ -838,25 +844,25 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45271.320214004627" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{00000000-000A-0000-FFFF-FFFF11000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45273.962201273149" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="40" xr:uid="{00000000-000A-0000-FFFF-FFFF11000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2023-12-11T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2023-12-14T00:00:00"/>
     </cacheField>
     <cacheField name="Winner" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.50600000000000001" maxValue="0.876"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.502" maxValue="0.876"/>
     </cacheField>
     <cacheField name="Loser" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Loser Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.124" maxValue="0.49399999999999999"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.124" maxValue="0.498"/>
     </cacheField>
     <cacheField name="Site" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -886,7 +892,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
   <r>
     <d v="2023-12-09T00:00:00"/>
     <s v="Boston Bruins"/>
@@ -1088,6 +1094,196 @@
     <x v="3"/>
   </r>
   <r>
+    <d v="2023-12-11T00:00:00"/>
+    <s v="Colorado Avalanche"/>
+    <n v="0.68799999999999994"/>
+    <s v="Calgary Flames"/>
+    <n v="0.312"/>
+    <s v="Playing At:  Colorado Avalanche   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-11T00:00:00"/>
+    <s v="Dallas Stars"/>
+    <n v="0.622"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.378"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-11T00:00:00"/>
+    <s v="Buffalo Sabres"/>
+    <n v="0.52200000000000002"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.47799999999999998"/>
+    <s v="Playing At:  Buffalo Sabres   Home"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-11T00:00:00"/>
+    <s v="Toronto Maple Leafs"/>
+    <n v="0.502"/>
+    <s v="New York Islanders"/>
+    <n v="0.498"/>
+    <s v="Playing At:  New York Islanders   Home"/>
+    <n v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Edmonton Oilers"/>
+    <n v="0.82399999999999995"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.17599999999999999"/>
+    <s v="Playing At:  Edmonton Oilers   Home"/>
+    <n v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Winnipeg Jets"/>
+    <n v="0.77800000000000002"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.222"/>
+    <s v="Playing At:  San Jose Sharks   Home"/>
+    <n v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Vegas Golden Knights"/>
+    <n v="0.69199999999999995"/>
+    <s v="Calgary Flames"/>
+    <n v="0.308"/>
+    <s v="Playing At:  Vegas Golden Knights   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Florida Panthers"/>
+    <n v="0.68200000000000005"/>
+    <s v="Seattle Kraken"/>
+    <n v="0.318"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Nashville Predators"/>
+    <n v="0.68"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.32"/>
+    <s v="Playing At:  Nashville Predators   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="New York Rangers"/>
+    <n v="0.65200000000000002"/>
+    <s v="Toronto Maple Leafs"/>
+    <n v="0.34799999999999998"/>
+    <s v="Playing At:  New York Rangers   Home"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Vancouver Canucks"/>
+    <n v="0.57199999999999995"/>
+    <s v="Tampa Bay Lightning"/>
+    <n v="0.42799999999999999"/>
+    <s v="Playing At:  Vancouver Canucks   Home"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Ottawa Senators"/>
+    <n v="0.56200000000000006"/>
+    <s v="Carolina Hurricanes"/>
+    <n v="0.438"/>
+    <s v="Playing At:  Ottawa Senators   Home"/>
+    <n v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="St. Louis Blues"/>
+    <n v="0.52200000000000002"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.47799999999999998"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <n v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-12T00:00:00"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.51600000000000001"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.48399999999999999"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-12-13T00:00:00"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.73"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.27"/>
+    <s v="Playing At:  Montreal Canadiens   Home"/>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2023-12-13T00:00:00"/>
+    <s v="New York Islanders"/>
+    <n v="0.624"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.376"/>
+    <s v="Playing At:  New York Islanders   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-13T00:00:00"/>
+    <s v="Colorado Avalanche"/>
+    <n v="0.622"/>
+    <s v="Buffalo Sabres"/>
+    <n v="0.378"/>
+    <s v="Playing At:  Colorado Avalanche   Home"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-13T00:00:00"/>
+    <s v="Boston Bruins"/>
+    <n v="0.622"/>
+    <s v="New Jersey Devils"/>
+    <n v="0.378"/>
+    <s v="Playing At:  New Jersey Devils   Home"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-12-13T00:00:00"/>
+    <s v="Los Angeles Kings"/>
+    <n v="0.56999999999999995"/>
+    <s v="Winnipeg Jets"/>
+    <n v="0.43"/>
+    <s v="Playing At:  Los Angeles Kings   Home"/>
+    <n v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -1101,7 +1297,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1472,21 +1668,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D10"/>
+  <dimension ref="A3:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>56</v>
       </c>
@@ -1499,8 +1696,11 @@
       <c r="D3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>66</v>
       </c>
@@ -1514,84 +1714,111 @@
         <f>C4/B4</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>SUM(B4:B6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
         <v>3</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" ref="D5:D9" si="0">C5/B5</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C4:C6)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
         <v>6</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="5">
+        <f>F5/F4</f>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="6">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="F8">
+        <f>SUM(B7:B8)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="6">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C9" s="6">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="F9">
+        <f>SUM(C7:C8)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="5"/>
+      <c r="F10" s="5">
+        <f>F9/F8</f>
+        <v>0.66666666666666663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1602,21 +1829,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45269</v>
       </c>
@@ -1668,7 +1895,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45269</v>
       </c>
@@ -1694,7 +1921,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45269</v>
       </c>
@@ -1720,7 +1947,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45269</v>
       </c>
@@ -1746,7 +1973,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45269</v>
       </c>
@@ -1772,7 +1999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45269</v>
       </c>
@@ -1798,7 +2025,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45269</v>
       </c>
@@ -1824,7 +2051,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45269</v>
       </c>
@@ -1850,7 +2077,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45269</v>
       </c>
@@ -1876,7 +2103,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45269</v>
       </c>
@@ -1902,7 +2129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45269</v>
       </c>
@@ -1928,7 +2155,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45269</v>
       </c>
@@ -1954,7 +2181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45270</v>
       </c>
@@ -1980,7 +2207,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45270</v>
       </c>
@@ -2006,7 +2233,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45270</v>
       </c>
@@ -2032,7 +2259,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45270</v>
       </c>
@@ -2058,7 +2285,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45270</v>
       </c>
@@ -2084,7 +2311,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45270</v>
       </c>
@@ -2110,7 +2337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45270</v>
       </c>
@@ -2136,7 +2363,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45270</v>
       </c>
@@ -2162,7 +2389,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45271</v>
       </c>
@@ -2180,13 +2407,16 @@
       </c>
       <c r="F22" t="s">
         <v>11</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
       </c>
       <c r="H22" t="str" cm="1">
         <f t="array" ref="H22">_xlfn.IFS(C22 &gt;= 0.85, "85  &lt;", AND(C22 &gt;=0.8, C22 &lt; 0.85), "80-85", AND(C22 &gt;= 0.7, C22 &lt; 0.8), "70-80", AND(C22 &gt;= 0.6, C22 &lt; 0.7),  "60-70", AND(C22 &gt;= 0.5, C22 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45271</v>
       </c>
@@ -2204,13 +2434,16 @@
       </c>
       <c r="F23" t="s">
         <v>32</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
       </c>
       <c r="H23" t="str" cm="1">
         <f t="array" ref="H23">_xlfn.IFS(C23 &gt;= 0.85, "85  &lt;", AND(C23 &gt;=0.8, C23 &lt; 0.85), "80-85", AND(C23 &gt;= 0.7, C23 &lt; 0.8), "70-80", AND(C23 &gt;= 0.6, C23 &lt; 0.7),  "60-70", AND(C23 &gt;= 0.5, C23 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45271</v>
       </c>
@@ -2228,13 +2461,16 @@
       </c>
       <c r="F24" t="s">
         <v>49</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
       </c>
       <c r="H24" t="str" cm="1">
         <f t="array" ref="H24">_xlfn.IFS(C24 &gt;= 0.85, "85  &lt;", AND(C24 &gt;=0.8, C24 &lt; 0.85), "80-85", AND(C24 &gt;= 0.7, C24 &lt; 0.8), "70-80", AND(C24 &gt;= 0.6, C24 &lt; 0.7),  "60-70", AND(C24 &gt;= 0.5, C24 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45271</v>
       </c>
@@ -2252,295 +2488,367 @@
       </c>
       <c r="F25" t="s">
         <v>43</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25" t="str" cm="1">
         <f t="array" ref="H25">_xlfn.IFS(C25 &gt;= 0.85, "85  &lt;", AND(C25 &gt;=0.8, C25 &lt; 0.85), "80-85", AND(C25 &gt;= 0.7, C25 &lt; 0.8), "70-80", AND(C25 &gt;= 0.6, C25 &lt; 0.7),  "60-70", AND(C25 &gt;= 0.5, C25 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="H26" t="e" cm="1">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45272</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="str" cm="1">
         <f t="array" ref="H26">_xlfn.IFS(C26 &gt;= 0.85, "85  &lt;", AND(C26 &gt;=0.8, C26 &lt; 0.85), "80-85", AND(C26 &gt;= 0.7, C26 &lt; 0.8), "70-80", AND(C26 &gt;= 0.6, C26 &lt; 0.7),  "60-70", AND(C26 &gt;= 0.5, C26 &lt; 0.6), "50-60")</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80-85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45272</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C27" s="2">
-        <v>0.82399999999999995</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E27" s="2">
-        <v>0.17599999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
       </c>
       <c r="H27" t="str" cm="1">
         <f t="array" ref="H27">_xlfn.IFS(C27 &gt;= 0.85, "85  &lt;", AND(C27 &gt;=0.8, C27 &lt; 0.85), "80-85", AND(C27 &gt;= 0.7, C27 &lt; 0.8), "70-80", AND(C27 &gt;= 0.6, C27 &lt; 0.7),  "60-70", AND(C27 &gt;= 0.5, C27 &lt; 0.6), "50-60")</f>
-        <v>80-85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45272</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2">
-        <v>0.77800000000000002</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E28" s="2">
-        <v>0.222</v>
+        <v>0.308</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
       </c>
       <c r="H28" t="str" cm="1">
         <f t="array" ref="H28">_xlfn.IFS(C28 &gt;= 0.85, "85  &lt;", AND(C28 &gt;=0.8, C28 &lt; 0.85), "80-85", AND(C28 &gt;= 0.7, C28 &lt; 0.8), "70-80", AND(C28 &gt;= 0.6, C28 &lt; 0.7),  "60-70", AND(C28 &gt;= 0.5, C28 &lt; 0.6), "50-60")</f>
-        <v>70-80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45272</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C29" s="2">
-        <v>0.69199999999999995</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E29" s="2">
-        <v>0.308</v>
+        <v>0.318</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29" t="str" cm="1">
         <f t="array" ref="H29">_xlfn.IFS(C29 &gt;= 0.85, "85  &lt;", AND(C29 &gt;=0.8, C29 &lt; 0.85), "80-85", AND(C29 &gt;= 0.7, C29 &lt; 0.8), "70-80", AND(C29 &gt;= 0.6, C29 &lt; 0.7),  "60-70", AND(C29 &gt;= 0.5, C29 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45272</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2">
-        <v>0.68200000000000005</v>
+        <v>0.68</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E30" s="2">
-        <v>0.318</v>
+        <v>0.32</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>68</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
       <c r="H30" t="str" cm="1">
         <f t="array" ref="H30">_xlfn.IFS(C30 &gt;= 0.85, "85  &lt;", AND(C30 &gt;=0.8, C30 &lt; 0.85), "80-85", AND(C30 &gt;= 0.7, C30 &lt; 0.8), "70-80", AND(C30 &gt;= 0.6, C30 &lt; 0.7),  "60-70", AND(C30 &gt;= 0.5, C30 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45272</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2">
-        <v>0.68</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2">
-        <v>0.32</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
       </c>
       <c r="H31" t="str" cm="1">
         <f t="array" ref="H31">_xlfn.IFS(C31 &gt;= 0.85, "85  &lt;", AND(C31 &gt;=0.8, C31 &lt; 0.85), "80-85", AND(C31 &gt;= 0.7, C31 &lt; 0.8), "70-80", AND(C31 &gt;= 0.6, C31 &lt; 0.7),  "60-70", AND(C31 &gt;= 0.5, C31 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45272</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C32" s="2">
-        <v>0.65200000000000002</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2">
-        <v>0.34799999999999998</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
       </c>
       <c r="H32" t="str" cm="1">
         <f t="array" ref="H32">_xlfn.IFS(C32 &gt;= 0.85, "85  &lt;", AND(C32 &gt;=0.8, C32 &lt; 0.85), "80-85", AND(C32 &gt;= 0.7, C32 &lt; 0.8), "70-80", AND(C32 &gt;= 0.6, C32 &lt; 0.7),  "60-70", AND(C32 &gt;= 0.5, C32 &lt; 0.6), "50-60")</f>
-        <v>60-70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45272</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2">
-        <v>0.57199999999999995</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E33" s="2">
-        <v>0.42799999999999999</v>
+        <v>0.438</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>69</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
       </c>
       <c r="H33" t="str" cm="1">
         <f t="array" ref="H33">_xlfn.IFS(C33 &gt;= 0.85, "85  &lt;", AND(C33 &gt;=0.8, C33 &lt; 0.85), "80-85", AND(C33 &gt;= 0.7, C33 &lt; 0.8), "70-80", AND(C33 &gt;= 0.6, C33 &lt; 0.7),  "60-70", AND(C33 &gt;= 0.5, C33 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45272</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C34" s="2">
-        <v>0.56200000000000006</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E34" s="2">
-        <v>0.438</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
       <c r="H34" t="str" cm="1">
         <f t="array" ref="H34">_xlfn.IFS(C34 &gt;= 0.85, "85  &lt;", AND(C34 &gt;=0.8, C34 &lt; 0.85), "80-85", AND(C34 &gt;= 0.7, C34 &lt; 0.8), "70-80", AND(C34 &gt;= 0.6, C34 &lt; 0.7),  "60-70", AND(C34 &gt;= 0.5, C34 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45272</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2">
-        <v>0.52200000000000002</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E35" s="2">
-        <v>0.47799999999999998</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="F35" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
       </c>
       <c r="H35" t="str" cm="1">
         <f t="array" ref="H35">_xlfn.IFS(C35 &gt;= 0.85, "85  &lt;", AND(C35 &gt;=0.8, C35 &lt; 0.85), "80-85", AND(C35 &gt;= 0.7, C35 &lt; 0.8), "70-80", AND(C35 &gt;= 0.6, C35 &lt; 0.7),  "60-70", AND(C35 &gt;= 0.5, C35 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>45272</v>
+        <v>45273</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="2">
-        <v>0.51600000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E36" s="2">
-        <v>0.48399999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
       </c>
       <c r="H36" t="str" cm="1">
         <f t="array" ref="H36">_xlfn.IFS(C36 &gt;= 0.85, "85  &lt;", AND(C36 &gt;=0.8, C36 &lt; 0.85), "80-85", AND(C36 &gt;= 0.7, C36 &lt; 0.8), "70-80", AND(C36 &gt;= 0.6, C36 &lt; 0.7),  "60-70", AND(C36 &gt;= 0.5, C36 &lt; 0.6), "50-60")</f>
-        <v>50-60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="C37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="H37" t="e" cm="1">
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>45273</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.624</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.376</v>
+      </c>
+      <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="str" cm="1">
         <f t="array" ref="H37">_xlfn.IFS(C37 &gt;= 0.85, "85  &lt;", AND(C37 &gt;=0.8, C37 &lt; 0.85), "80-85", AND(C37 &gt;= 0.7, C37 &lt; 0.8), "70-80", AND(C37 &gt;= 0.6, C37 &lt; 0.7),  "60-70", AND(C37 &gt;= 0.5, C37 &lt; 0.6), "50-60")</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45273</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="C38" s="2">
-        <v>0.73</v>
+        <v>0.622</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E38" s="2">
-        <v>0.27</v>
+        <v>0.378</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
       </c>
       <c r="H38" t="str" cm="1">
         <f t="array" ref="H38">_xlfn.IFS(C38 &gt;= 0.85, "85  &lt;", AND(C38 &gt;=0.8, C38 &lt; 0.85), "80-85", AND(C38 &gt;= 0.7, C38 &lt; 0.8), "70-80", AND(C38 &gt;= 0.6, C38 &lt; 0.7),  "60-70", AND(C38 &gt;= 0.5, C38 &lt; 0.6), "50-60")</f>
-        <v>70-80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45273</v>
       </c>
@@ -2558,13 +2866,16 @@
       </c>
       <c r="F39" t="s">
         <v>73</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
       </c>
       <c r="H39" t="str" cm="1">
         <f t="array" ref="H39">_xlfn.IFS(C39 &gt;= 0.85, "85  &lt;", AND(C39 &gt;=0.8, C39 &lt; 0.85), "80-85", AND(C39 &gt;= 0.7, C39 &lt; 0.8), "70-80", AND(C39 &gt;= 0.6, C39 &lt; 0.7),  "60-70", AND(C39 &gt;= 0.5, C39 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45273</v>
       </c>
@@ -2582,6 +2893,9 @@
       </c>
       <c r="F40" t="s">
         <v>74</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
       <c r="H40" t="str" cm="1">
         <f t="array" ref="H40">_xlfn.IFS(C40 &gt;= 0.85, "85  &lt;", AND(C40 &gt;=0.8, C40 &lt; 0.85), "80-85", AND(C40 &gt;= 0.7, C40 &lt; 0.8), "70-80", AND(C40 &gt;= 0.6, C40 &lt; 0.7),  "60-70", AND(C40 &gt;= 0.5, C40 &lt; 0.6), "50-60")</f>
@@ -2589,18 +2903,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C22:C40">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E25 E27:E36 E38:E40">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="E22:E35">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2611,6 +2915,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C35">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>